<commit_message>
cosmic test cases, cravat_to_vcf
</commit_message>
<xml_diff>
--- a/test_cases/#testCases.xlsx
+++ b/test_cases/#testCases.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="70">
   <si>
     <t>Column</t>
   </si>
@@ -223,6 +223,12 @@
   </si>
   <si>
     <t>identical samps in study</t>
+  </si>
+  <si>
+    <t>cosmic</t>
+  </si>
+  <si>
+    <t>include in cosmic? database needs updating</t>
   </si>
 </sst>
 </file>
@@ -574,405 +580,459 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D59"/>
+  <dimension ref="A1:E59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C46" sqref="C46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>20</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>23</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
         <v>1</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
-        <v>21</v>
-      </c>
       <c r="C3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
         <v>3</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
-        <v>21</v>
-      </c>
       <c r="C5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
-        <v>21</v>
-      </c>
       <c r="C7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
         <v>7</v>
       </c>
-      <c r="B8" t="s">
-        <v>21</v>
-      </c>
       <c r="C8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
         <v>8</v>
       </c>
-      <c r="B9" t="s">
-        <v>21</v>
-      </c>
       <c r="C9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
         <v>9</v>
       </c>
-      <c r="B10" t="s">
-        <v>21</v>
-      </c>
       <c r="C10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>1</v>
+      </c>
+      <c r="B11" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
         <v>11</v>
       </c>
-      <c r="B12" t="s">
-        <v>21</v>
-      </c>
       <c r="C12" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
         <v>12</v>
       </c>
-      <c r="B13" t="s">
-        <v>21</v>
-      </c>
       <c r="C13" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
         <v>13</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E14" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
         <v>14</v>
       </c>
-      <c r="B15" t="s">
-        <v>21</v>
-      </c>
       <c r="C15" t="s">
+        <v>21</v>
+      </c>
+      <c r="D15" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
         <v>16</v>
       </c>
-      <c r="B17" t="s">
-        <v>21</v>
-      </c>
       <c r="C17" t="s">
+        <v>21</v>
+      </c>
+      <c r="D17" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
         <v>17</v>
       </c>
-      <c r="B18" t="s">
-        <v>21</v>
-      </c>
       <c r="C18" t="s">
+        <v>21</v>
+      </c>
+      <c r="D18" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
         <v>18</v>
       </c>
-      <c r="B19" t="s">
-        <v>21</v>
-      </c>
       <c r="C19" t="s">
+        <v>21</v>
+      </c>
+      <c r="D19" t="s">
         <v>28</v>
       </c>
-      <c r="D19" t="s">
+      <c r="E19" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>1</v>
+      </c>
+      <c r="B37" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>1</v>
+      </c>
+      <c r="B38" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
+      <c r="C39" t="s">
+        <v>21</v>
+      </c>
+      <c r="D39" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
+      <c r="E40" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
+      <c r="E41" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
+      <c r="C42" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
+      <c r="E43" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B44" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B45" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B46" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B47" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>2</v>
+      </c>
+      <c r="B48" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>2</v>
+      </c>
+      <c r="B49" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>2</v>
+      </c>
+      <c r="B50" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>2</v>
+      </c>
+      <c r="B51" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>2</v>
+      </c>
+      <c r="B52" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>2</v>
+      </c>
+      <c r="B53" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>2</v>
+      </c>
+      <c r="B54" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>2</v>
+      </c>
+      <c r="B55" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>2</v>
+      </c>
+      <c r="B56" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B57" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B58" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B59" t="s">
         <v>67</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added parsing of db result, added exac case
</commit_message>
<xml_diff>
--- a/test_cases/#testCases.xlsx
+++ b/test_cases/#testCases.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="74">
   <si>
     <t>Column</t>
   </si>
@@ -229,6 +229,18 @@
   </si>
   <si>
     <t>include in cosmic? database needs updating</t>
+  </si>
+  <si>
+    <t>not full string, just prot change part</t>
+  </si>
+  <si>
+    <t>could be bug, mix up btwn variant reads, sample reads</t>
+  </si>
+  <si>
+    <t>exac</t>
+  </si>
+  <si>
+    <t>failing hard</t>
   </si>
 </sst>
 </file>
@@ -582,8 +594,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C46" sqref="C46"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E48" sqref="E48:E56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -748,8 +760,11 @@
       <c r="B16" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E16" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>16</v>
       </c>
@@ -759,8 +774,11 @@
       <c r="D17" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E17" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>17</v>
       </c>
@@ -771,7 +789,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>18</v>
       </c>
@@ -785,67 +803,73 @@
         <v>29</v>
       </c>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>3</v>
+      </c>
       <c r="B20" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>3</v>
+      </c>
       <c r="B21" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>30</v>
       </c>
@@ -872,7 +896,7 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B37" t="s">
         <v>35</v>
@@ -880,7 +904,7 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B38" t="s">
         <v>36</v>
@@ -920,13 +944,22 @@
       <c r="C42" t="s">
         <v>21</v>
       </c>
+      <c r="D42" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
         <v>41</v>
       </c>
+      <c r="C43" t="s">
+        <v>21</v>
+      </c>
+      <c r="D43" t="s">
+        <v>68</v>
+      </c>
       <c r="E43" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
@@ -951,87 +984,168 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B48" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C48" t="s">
+        <v>21</v>
+      </c>
+      <c r="D48" t="s">
+        <v>72</v>
+      </c>
+      <c r="E48" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B49" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C49" t="s">
+        <v>21</v>
+      </c>
+      <c r="D49" t="s">
+        <v>72</v>
+      </c>
+      <c r="E49" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B50" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C50" t="s">
+        <v>21</v>
+      </c>
+      <c r="D50" t="s">
+        <v>72</v>
+      </c>
+      <c r="E50" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B51" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C51" t="s">
+        <v>21</v>
+      </c>
+      <c r="D51" t="s">
+        <v>72</v>
+      </c>
+      <c r="E51" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B52" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C52" t="s">
+        <v>21</v>
+      </c>
+      <c r="D52" t="s">
+        <v>72</v>
+      </c>
+      <c r="E52" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B53" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C53" t="s">
+        <v>21</v>
+      </c>
+      <c r="D53" t="s">
+        <v>72</v>
+      </c>
+      <c r="E53" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B54" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C54" t="s">
+        <v>21</v>
+      </c>
+      <c r="D54" t="s">
+        <v>72</v>
+      </c>
+      <c r="E54" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B55" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C55" t="s">
+        <v>21</v>
+      </c>
+      <c r="D55" t="s">
+        <v>72</v>
+      </c>
+      <c r="E55" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B56" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C56" t="s">
+        <v>21</v>
+      </c>
+      <c r="D56" t="s">
+        <v>72</v>
+      </c>
+      <c r="E56" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
         <v>67</v>
       </c>

</xml_diff>